<commit_message>
updated the zip file
</commit_message>
<xml_diff>
--- a/excels/priyanka/Announcement Mailer_EV-Graph.xlsx
+++ b/excels/priyanka/Announcement Mailer_EV-Graph.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eninrac\Desktop\Reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eninrac\ecosystem-mailer\ecosystem-announcement-mailer-template\excels\priyanka\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10EEA0EA-83BB-4E3B-BD60-0960B2877C07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87224A6C-721C-4A80-B4D2-CFB2F9CAA602}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="reportTable" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t>Maker Month Wise Data  For All State (2025)</t>
   </si>
@@ -37,114 +37,57 @@
     <t/>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>AUDI AG</t>
   </si>
   <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>BMW INDIA PVT LTD</t>
   </si>
   <si>
-    <t>3</t>
-  </si>
-  <si>
     <t>BYD INDIA PRIVATE LIMITED</t>
   </si>
   <si>
-    <t>4</t>
-  </si>
-  <si>
     <t>HYUNDAI MOTOR INDIA LTD</t>
   </si>
   <si>
-    <t>5</t>
-  </si>
-  <si>
     <t>JAGUAR LAND ROVER INDIA LIMITED</t>
   </si>
   <si>
-    <t>6</t>
-  </si>
-  <si>
     <t>KIA INDIA PRIVATE LIMITED</t>
   </si>
   <si>
-    <t>7</t>
-  </si>
-  <si>
     <t>MAHINDRA ELECTRIC AUTOMOBILE LTD</t>
   </si>
   <si>
-    <t>8</t>
-  </si>
-  <si>
     <t>MAHINDRA &amp; MAHINDRA LIMITED</t>
   </si>
   <si>
-    <t>9</t>
-  </si>
-  <si>
     <t>MERCEDES -BENZ AG</t>
   </si>
   <si>
-    <t>10</t>
-  </si>
-  <si>
     <t>MERCEDES-BENZ INDIA PVT LTD</t>
   </si>
   <si>
-    <t>11</t>
-  </si>
-  <si>
     <t>MG MOTOR INDIA PVT LTD</t>
   </si>
   <si>
-    <t>12</t>
-  </si>
-  <si>
     <t>PCA AUTOMOBILES INDIA PVT LTD</t>
   </si>
   <si>
-    <t>13</t>
-  </si>
-  <si>
     <t>PORSCHE AG GERMANY</t>
   </si>
   <si>
-    <t>14</t>
-  </si>
-  <si>
     <t>ROLLS ROYCE MOTOR (IMPORTER: KUN MOTOR)</t>
   </si>
   <si>
-    <t>15</t>
-  </si>
-  <si>
     <t>SWITCH MOBILITY AUTOMOTIVE LTD</t>
   </si>
   <si>
-    <t>16</t>
-  </si>
-  <si>
     <t>TATA MOTORS LTD</t>
   </si>
   <si>
-    <t>17</t>
-  </si>
-  <si>
     <t>TATA MOTORS PASSENGER VEHICLES LTD</t>
   </si>
   <si>
-    <t>18</t>
-  </si>
-  <si>
     <t>TATA PASSENGER ELECTRIC MOBILITY LTD</t>
   </si>
   <si>
@@ -191,9 +134,6 @@
   </si>
   <si>
     <t>JLR</t>
-  </si>
-  <si>
-    <t>Units</t>
   </si>
   <si>
     <t>Total</t>
@@ -226,15 +166,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -251,21 +197,205 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -461,7 +591,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>reportTable!$F$4:$F$17</c:f>
+              <c:f>reportTable!$G$3:$G$16</c:f>
               <c:strCache>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
@@ -511,7 +641,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>reportTable!$G$4:$G$17</c:f>
+              <c:f>reportTable!$H$3:$H$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -1321,15 +1451,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>447676</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>152401</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1357,9 +1487,9 @@
   </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1008802" cy="248145"/>
@@ -1429,15 +1559,15 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2068,372 +2198,363 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G23"/>
+  <dimension ref="B1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" zoomScale="53" workbookViewId="0">
+      <selection activeCell="U26" sqref="U26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.5703125" customWidth="1"/>
+    <col min="2" max="2" width="4.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C3" s="1"/>
-      <c r="F3" s="1" t="s">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B3" s="10">
+        <v>1</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="12">
+        <v>5055</v>
+      </c>
+      <c r="G3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B4" s="13">
         <v>2</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>57</v>
+      <c r="C4" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="15">
+        <v>4271</v>
+      </c>
+      <c r="G4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4">
+        <v>184</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C4" s="2">
-        <v>5055</v>
-      </c>
-      <c r="F4" t="s">
-        <v>53</v>
-      </c>
-      <c r="G4">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B5" s="13">
+        <v>3</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="16">
+        <v>672</v>
+      </c>
+      <c r="G5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B6" s="13">
+        <v>4</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="16">
+        <v>323</v>
+      </c>
+      <c r="G6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B7" s="13">
+        <v>5</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="16">
+        <v>316</v>
+      </c>
+      <c r="G7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B8" s="13">
+        <v>6</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="16">
+        <v>269</v>
+      </c>
+      <c r="G8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" s="2">
+        <v>4271</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B9" s="13">
+        <v>7</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="16">
+        <v>184</v>
+      </c>
+      <c r="G9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B10" s="13">
+        <v>8</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="16">
+        <v>69</v>
+      </c>
+      <c r="G10" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10">
+        <f>D14+D5</f>
+        <v>693</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B11" s="13">
+        <v>9</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="16">
+        <v>48</v>
+      </c>
+      <c r="G11" t="s">
+        <v>31</v>
+      </c>
+      <c r="H11">
+        <f>D10+D12</f>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B12" s="13">
+        <v>10</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="16">
+        <v>27</v>
+      </c>
+      <c r="G12" t="s">
+        <v>29</v>
+      </c>
+      <c r="H12">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B13" s="13">
+        <v>11</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="16">
+        <v>27</v>
+      </c>
+      <c r="G13" t="s">
+        <v>35</v>
+      </c>
+      <c r="H13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B14" s="13">
+        <v>12</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="16">
+        <v>21</v>
+      </c>
+      <c r="G14" t="s">
+        <v>36</v>
+      </c>
+      <c r="H14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B15" s="13">
+        <v>13</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="16">
         <v>19</v>
       </c>
+      <c r="G15" t="s">
+        <v>24</v>
+      </c>
+      <c r="H15" s="2">
+        <f>D16+D3</f>
+        <v>5071</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B16" s="13">
+        <v>14</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="16">
+        <v>16</v>
+      </c>
+      <c r="G16" t="s">
+        <v>33</v>
+      </c>
+      <c r="H16">
         <v>27</v>
       </c>
-      <c r="C5" s="2">
-        <v>4271</v>
-      </c>
-      <c r="F5" t="s">
-        <v>49</v>
-      </c>
-      <c r="G5">
-        <v>184</v>
-      </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B17" s="13">
+        <v>15</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="16">
+        <v>6</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H17" s="3">
+        <v>11328</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B18" s="13">
+        <v>16</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B19" s="13">
+        <v>17</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B20" s="13">
+        <v>18</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B21" s="13">
+        <v>19</v>
+      </c>
+      <c r="C21" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6">
-        <v>672</v>
-      </c>
-      <c r="F6" t="s">
-        <v>47</v>
-      </c>
-      <c r="G6">
-        <v>316</v>
+      <c r="D21" s="16">
+        <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7">
-        <v>323</v>
-      </c>
-      <c r="F7" t="s">
-        <v>46</v>
-      </c>
-      <c r="G7">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8">
-        <v>316</v>
-      </c>
-      <c r="F8" t="s">
-        <v>56</v>
-      </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9">
-        <v>269</v>
-      </c>
-      <c r="F9" t="s">
-        <v>44</v>
-      </c>
-      <c r="G9" s="2">
-        <v>4271</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10">
-        <v>184</v>
-      </c>
-      <c r="F10" t="s">
-        <v>51</v>
-      </c>
-      <c r="G10">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11">
-        <v>69</v>
-      </c>
-      <c r="F11" t="s">
-        <v>45</v>
-      </c>
-      <c r="G11">
-        <f>C15+C6</f>
-        <v>693</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12">
-        <v>48</v>
-      </c>
-      <c r="F12" t="s">
-        <v>50</v>
-      </c>
-      <c r="G12">
-        <f>C11+C13</f>
-        <v>96</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13">
-        <v>27</v>
-      </c>
-      <c r="F13" t="s">
-        <v>48</v>
-      </c>
-      <c r="G13">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14">
-        <v>27</v>
-      </c>
-      <c r="F14" t="s">
-        <v>54</v>
-      </c>
-      <c r="G14">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15">
-        <v>21</v>
-      </c>
-      <c r="F15" t="s">
-        <v>55</v>
-      </c>
-      <c r="G15">
+    <row r="22" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B22" s="17" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16">
-        <v>19</v>
-      </c>
-      <c r="F16" t="s">
-        <v>43</v>
-      </c>
-      <c r="G16" s="2">
-        <f>C17+C4</f>
-        <v>5071</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="C22" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="B17" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17">
-        <v>16</v>
-      </c>
-      <c r="F17" t="s">
-        <v>52</v>
-      </c>
-      <c r="G17">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" t="s">
-        <v>31</v>
-      </c>
-      <c r="C18">
-        <v>6</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="G18" s="4">
-        <v>11328</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>34</v>
-      </c>
-      <c r="B21" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>36</v>
-      </c>
-      <c r="B22" t="s">
-        <v>37</v>
-      </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>4</v>
-      </c>
-      <c r="B23" t="s">
-        <v>4</v>
-      </c>
-      <c r="C23" s="2">
-        <f>SUM(C4:C22)</f>
+      <c r="D22" s="19">
+        <f>SUM(D3:D21)</f>
         <v>11330</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F4:G17">
-    <sortCondition ref="F4:F17"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="G3:H16">
+    <sortCondition ref="G3:G16"/>
   </sortState>
   <mergeCells count="1">
-    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="B1:F1"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>